<commit_message>
Added compatibility with relative line references (e.g. line=+12) in <location> tags.
</commit_message>
<xml_diff>
--- a/tests/files/scenario_multilocation.xlsx
+++ b/tests/files/scenario_multilocation.xlsx
@@ -64,7 +64,7 @@
     <t/>
   </si>
   <si>
-    <t>../themewidget.cpp - 289</t>
+    <t>../themewidget.cpp - +289</t>
   </si>
   <si>
     <t>../themewidget.cpp - 290</t>
@@ -85,7 +85,7 @@
     <t>../themewidget.cpp - 90</t>
   </si>
   <si>
-    <t>../themewidget.cpp - 91</t>
+    <t>../themewidget.cpp - -91</t>
   </si>
   <si>
     <t>ThemeWidgetForm</t>

</xml_diff>